<commit_message>
Data has been added.
</commit_message>
<xml_diff>
--- a/presurvey.xlsx
+++ b/presurvey.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Household" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t xml:space="preserve">Income </t>
   </si>
@@ -33,6 +33,15 @@
   </si>
   <si>
     <t>HhID</t>
+  </si>
+  <si>
+    <t>50 000</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>m</t>
   </si>
 </sst>
 </file>
@@ -350,10 +359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -369,6 +378,39 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>102</v>
+      </c>
+      <c r="B3">
+        <v>45000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>103</v>
+      </c>
+      <c r="B4">
+        <v>78000</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>